<commit_message>
Proyecto trimestral: interfaz gráfica avanzada, registro de usuarios, productos, edición de usuarios, módulo de caja y asignación de base realizado. Faltan corrección de errores
</commit_message>
<xml_diff>
--- a/src/services/file/products.xlsx
+++ b/src/services/file/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Swyme\Desktop\proyecto-semestral\src\services\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9234A830-12BF-4AB0-ACDC-C76A2F1058C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743A3D7E-6BEA-4B18-8CE7-27E5F4A2D517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{745FBC98-7909-43A2-9ED3-EBC8572D50C5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>cod_articulo</t>
   </si>
@@ -48,25 +48,61 @@
     <t>iva_producto</t>
   </si>
   <si>
-    <t xml:space="preserve">0001 </t>
-  </si>
-  <si>
     <t>vencimiento_producto</t>
   </si>
   <si>
-    <t>Leche</t>
-  </si>
-  <si>
     <t>0002</t>
   </si>
   <si>
-    <t>Cocacola</t>
-  </si>
-  <si>
-    <t>23-06-2023</t>
-  </si>
-  <si>
-    <t>15-04-2022</t>
+    <t>disponibilidad</t>
+  </si>
+  <si>
+    <t>categoria</t>
+  </si>
+  <si>
+    <t>Arbeja</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2022-10-25</t>
+  </si>
+  <si>
+    <t>0001</t>
+  </si>
+  <si>
+    <t>Frijol</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>2023-11-22</t>
+  </si>
+  <si>
+    <t>0003</t>
+  </si>
+  <si>
+    <t>Garbanzo</t>
+  </si>
+  <si>
+    <t>4000</t>
+  </si>
+  <si>
+    <t>40</t>
   </si>
 </sst>
 </file>
@@ -102,16 +138,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -427,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCD8CB2-3001-4253-AE3B-06D3C322B059}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,64 +470,106 @@
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2600</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1">
-        <v>3500</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>9</v>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A2:A3" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Proyecto trimestral: proceso de facturación completado. Bug's pendientes
</commit_message>
<xml_diff>
--- a/src/services/file/products.xlsx
+++ b/src/services/file/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Swyme\Desktop\proyecto-semestral\src\services\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743A3D7E-6BEA-4B18-8CE7-27E5F4A2D517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5456DA-AAFD-402A-97E5-4EC864830F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{745FBC98-7909-43A2-9ED3-EBC8572D50C5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>cod_articulo</t>
   </si>
@@ -103,6 +103,54 @@
   </si>
   <si>
     <t>40</t>
+  </si>
+  <si>
+    <t>0004</t>
+  </si>
+  <si>
+    <t>Cocacola</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>3500</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>2024-09-11</t>
+  </si>
+  <si>
+    <t>0005</t>
+  </si>
+  <si>
+    <t>Colombiana</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>2800</t>
+  </si>
+  <si>
+    <t>2024-10-25</t>
+  </si>
+  <si>
+    <t>0006</t>
+  </si>
+  <si>
+    <t>Margaritas</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>2021-11-20</t>
   </si>
 </sst>
 </file>
@@ -458,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCD8CB2-3001-4253-AE3B-06D3C322B059}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,6 +617,75 @@
         <v>18</v>
       </c>
     </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Proyecto trimestral: tipo de pago por bancos, cierre de caja completo, asignación de base y creación de cajas.
</commit_message>
<xml_diff>
--- a/src/services/file/products.xlsx
+++ b/src/services/file/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Swyme\Desktop\proyecto-semestral\src\services\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5456DA-AAFD-402A-97E5-4EC864830F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B903B9-2956-4E32-B0AF-DE3D28F84D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{745FBC98-7909-43A2-9ED3-EBC8572D50C5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>cod_articulo</t>
   </si>
@@ -87,9 +87,6 @@
     <t>2000</t>
   </si>
   <si>
-    <t>50</t>
-  </si>
-  <si>
     <t>2023-11-22</t>
   </si>
   <si>
@@ -102,9 +99,6 @@
     <t>4000</t>
   </si>
   <si>
-    <t>40</t>
-  </si>
-  <si>
     <t>0004</t>
   </si>
   <si>
@@ -114,9 +108,6 @@
     <t>500</t>
   </si>
   <si>
-    <t>3500</t>
-  </si>
-  <si>
     <t>19</t>
   </si>
   <si>
@@ -135,9 +126,6 @@
     <t>300</t>
   </si>
   <si>
-    <t>2800</t>
-  </si>
-  <si>
     <t>2024-10-25</t>
   </si>
   <si>
@@ -151,6 +139,12 @@
   </si>
   <si>
     <t>2021-11-20</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>600</t>
   </si>
 </sst>
 </file>
@@ -508,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCD8CB2-3001-4253-AE3B-06D3C322B059}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,7 +575,7 @@
         <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>11</v>
@@ -590,22 +584,22 @@
         <v>12</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>11</v>
@@ -614,67 +608,67 @@
         <v>12</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>11</v>
@@ -683,7 +677,7 @@
         <v>12</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>